<commit_message>
adding adult TPC scripts and data files
</commit_message>
<xml_diff>
--- a/RAnalysis/data/TPC/RampSettings.xlsx
+++ b/RAnalysis/data/TPC/RampSettings.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hputnam/MyProjects/Poc_RAPID/RAnalysis/data/TPC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F630A62-16A3-B940-844B-3AB5FC2EABDC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE69B472-E96A-C942-9557-471EB16DCA87}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="10000" windowHeight="14820" xr2:uid="{05019E3E-6BD5-B64B-A53F-DABBA1D9AA2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>

</xml_diff>

<commit_message>
adding recruit TPC scripts and data files Run4
</commit_message>
<xml_diff>
--- a/RAnalysis/data/TPC/RampSettings.xlsx
+++ b/RAnalysis/data/TPC/RampSettings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hputnam/MyProjects/Poc_RAPID/RAnalysis/data/TPC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE69B472-E96A-C942-9557-471EB16DCA87}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C52BF15-DE9E-EB46-8623-DBF036FBE27B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="10000" windowHeight="14820" xr2:uid="{05019E3E-6BD5-B64B-A53F-DABBA1D9AA2C}"/>
   </bookViews>
@@ -395,14 +395,14 @@
   <dimension ref="B1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E1" s="1">
-        <v>0.55208333333333337</v>
+        <v>0.54583333333333328</v>
       </c>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
@@ -417,7 +417,7 @@
       </c>
       <c r="E2" s="1">
         <f>E1+D2</f>
-        <v>0.5625</v>
+        <v>0.55624999999999991</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
@@ -432,7 +432,7 @@
       </c>
       <c r="E3" s="1">
         <f>E2+D3</f>
-        <v>0.57291666666666663</v>
+        <v>0.56666666666666654</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
@@ -443,7 +443,7 @@
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="E4" s="1">
-        <v>0.58819444444444446</v>
+        <v>0.58888888888888891</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
@@ -458,7 +458,7 @@
       </c>
       <c r="E5" s="1">
         <f t="shared" ref="E5:E24" si="0">E4+D5</f>
-        <v>0.59861111111111109</v>
+        <v>0.59930555555555554</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
@@ -473,7 +473,7 @@
       </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>0.60902777777777772</v>
+        <v>0.60972222222222217</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
@@ -485,7 +485,7 @@
       </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>0.61597222222222214</v>
+        <v>0.61666666666666659</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
@@ -500,7 +500,7 @@
       </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>0.62638888888888877</v>
+        <v>0.62708333333333321</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
@@ -515,7 +515,7 @@
       </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>0.6368055555555554</v>
+        <v>0.63749999999999984</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
@@ -527,7 +527,7 @@
       </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>0.64374999999999982</v>
+        <v>0.64444444444444426</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
@@ -542,7 +542,7 @@
       </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>0.65416666666666645</v>
+        <v>0.65486111111111089</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
@@ -557,7 +557,7 @@
       </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>0.66458333333333308</v>
+        <v>0.66527777777777752</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
@@ -569,7 +569,7 @@
       </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>0.6715277777777775</v>
+        <v>0.67222222222222194</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
@@ -584,7 +584,7 @@
       </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>0.68194444444444413</v>
+        <v>0.68263888888888857</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
@@ -599,7 +599,7 @@
       </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>0.69236111111111076</v>
+        <v>0.6930555555555552</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
@@ -610,8 +610,7 @@
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="E16" s="1">
-        <f t="shared" si="0"/>
-        <v>0.69930555555555518</v>
+        <v>0.76250000000000007</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
@@ -626,7 +625,7 @@
       </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>0.70972222222222181</v>
+        <v>0.7729166666666667</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
@@ -641,7 +640,7 @@
       </c>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>0.72013888888888844</v>
+        <v>0.78333333333333333</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
@@ -652,8 +651,7 @@
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="E19" s="1">
-        <f t="shared" si="0"/>
-        <v>0.72708333333333286</v>
+        <v>0.8041666666666667</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
@@ -668,7 +666,7 @@
       </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>0.73749999999999949</v>
+        <v>0.81458333333333333</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
@@ -683,7 +681,7 @@
       </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>0.74791666666666612</v>
+        <v>0.82499999999999996</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
@@ -695,7 +693,7 @@
       </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>0.75486111111111054</v>
+        <v>0.83194444444444438</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
@@ -710,7 +708,7 @@
       </c>
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>0.76527777777777717</v>
+        <v>0.84236111111111101</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
@@ -725,7 +723,7 @@
       </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>0.7756944444444438</v>
+        <v>0.85277777777777763</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
temperature ramp data Run 5
</commit_message>
<xml_diff>
--- a/RAnalysis/data/TPC/RampSettings.xlsx
+++ b/RAnalysis/data/TPC/RampSettings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hputnam/MyProjects/Poc_RAPID/RAnalysis/data/TPC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C52BF15-DE9E-EB46-8623-DBF036FBE27B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C721C82C-2429-424D-B7F9-980F9F18D877}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="10000" windowHeight="14820" xr2:uid="{05019E3E-6BD5-B64B-A53F-DABBA1D9AA2C}"/>
   </bookViews>
@@ -395,7 +395,7 @@
   <dimension ref="B1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -443,7 +443,7 @@
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="E4" s="1">
-        <v>0.58888888888888891</v>
+        <v>0.56597222222222221</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
@@ -458,7 +458,7 @@
       </c>
       <c r="E5" s="1">
         <f t="shared" ref="E5:E24" si="0">E4+D5</f>
-        <v>0.59930555555555554</v>
+        <v>0.57638888888888884</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
@@ -473,7 +473,7 @@
       </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>0.60972222222222217</v>
+        <v>0.58680555555555547</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
@@ -484,8 +484,7 @@
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" si="0"/>
-        <v>0.61666666666666659</v>
+        <v>0.59930555555555554</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
@@ -500,7 +499,7 @@
       </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>0.62708333333333321</v>
+        <v>0.60972222222222217</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
@@ -515,7 +514,7 @@
       </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>0.63749999999999984</v>
+        <v>0.6201388888888888</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
@@ -527,7 +526,7 @@
       </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>0.64444444444444426</v>
+        <v>0.62708333333333321</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
@@ -542,7 +541,7 @@
       </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>0.65486111111111089</v>
+        <v>0.63749999999999984</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
@@ -557,7 +556,7 @@
       </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>0.66527777777777752</v>
+        <v>0.64791666666666647</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
@@ -569,7 +568,7 @@
       </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>0.67222222222222194</v>
+        <v>0.65486111111111089</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
@@ -584,7 +583,7 @@
       </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>0.68263888888888857</v>
+        <v>0.66527777777777752</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
@@ -599,7 +598,7 @@
       </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>0.6930555555555552</v>
+        <v>0.67569444444444415</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
@@ -610,7 +609,7 @@
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="E16" s="1">
-        <v>0.76250000000000007</v>
+        <v>0.70000000000000007</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
@@ -625,7 +624,7 @@
       </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>0.7729166666666667</v>
+        <v>0.7104166666666667</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
@@ -640,7 +639,7 @@
       </c>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>0.78333333333333333</v>
+        <v>0.72083333333333333</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
@@ -651,7 +650,8 @@
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="E19" s="1">
-        <v>0.8041666666666667</v>
+        <f t="shared" si="0"/>
+        <v>0.72777777777777775</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
@@ -666,7 +666,7 @@
       </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>0.81458333333333333</v>
+        <v>0.73819444444444438</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
@@ -681,7 +681,7 @@
       </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>0.82499999999999996</v>
+        <v>0.74861111111111101</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
@@ -693,7 +693,7 @@
       </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>0.83194444444444438</v>
+        <v>0.75555555555555542</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
@@ -708,7 +708,7 @@
       </c>
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>0.84236111111111101</v>
+        <v>0.76597222222222205</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
@@ -723,7 +723,7 @@
       </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>0.85277777777777763</v>
+        <v>0.77638888888888868</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">

</xml_diff>